<commit_message>
committing the changes done till reading file
</commit_message>
<xml_diff>
--- a/mapping_iris.xlsx
+++ b/mapping_iris.xlsx
@@ -5,20 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai Prashanth T S\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai Prashanth T S\Desktop\Learnings\python-mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78185963-C99D-4F0E-A63B-037E907233A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CBFBC9-619E-417C-9439-090E22DC9C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1BFD56FF-65B6-4578-9371-23171E477F86}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Complex_Logic" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
-  <si>
-    <t>mapping_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>src_file_name</t>
   </si>
@@ -204,13 +199,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,216 +527,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A32043-9C27-4626-8B1C-43342643AAF1}">
   <dimension ref="C4:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:J13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="5">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="4">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="4">
         <v>8</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="5">
-        <v>2</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="5">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="5">
-        <v>4</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="5">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="5">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="5">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="5">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E25" s="3"/>
+      <c r="E25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -753,198 +745,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29054B3-8C1F-4509-A5BE-F07BD63233A9}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4F1DF3-C914-4924-8525-0C5EC5AED836}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -962,39 +762,39 @@
   <sheetData>
     <row r="1" spans="1:6" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>